<commit_message>
Added 1 test case
</commit_message>
<xml_diff>
--- a/com.apartments/testdata/test_data.xlsx
+++ b/com.apartments/testdata/test_data.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdul\IdeaProjects\SeleniumBootcamp\com.apartments\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4235C879-4042-450E-8B17-24EE246B002C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D157C418-5F4F-45E1-8F47-4CDF0FE36E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="2565" windowWidth="16200" windowHeight="9308" activeTab="2" xr2:uid="{15BB0DDE-0818-4DE4-BF4F-9A0B827D75DD}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="2" activeTab="4" xr2:uid="{15BB0DDE-0818-4DE4-BF4F-9A0B827D75DD}"/>
   </bookViews>
   <sheets>
     <sheet name="login_crm" sheetId="1" r:id="rId1"/>
-    <sheet name="createContact_crm" sheetId="3" r:id="rId2"/>
-    <sheet name="signup_aparments.com" sheetId="2" r:id="rId3"/>
+    <sheet name="createContact_crm1" sheetId="3" r:id="rId2"/>
+    <sheet name="createContact_crm" sheetId="6" r:id="rId3"/>
+    <sheet name="signup_aparments.com" sheetId="2" r:id="rId4"/>
+    <sheet name="Signin_apartments" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="53">
   <si>
     <t>email</t>
   </si>
@@ -170,6 +172,33 @@
   </si>
   <si>
     <t>NY</t>
+  </si>
+  <si>
+    <t>first name</t>
+  </si>
+  <si>
+    <t>last name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abdullah </t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>12346</t>
+  </si>
+  <si>
+    <t>anoor1@gmail.com</t>
+  </si>
+  <si>
+    <t>anoor2@gmail.com</t>
+  </si>
+  <si>
+    <t>anoor3@gmail.com</t>
+  </si>
+  <si>
+    <t>Piit123!</t>
   </si>
 </sst>
 </file>
@@ -214,9 +243,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -581,7 +611,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -731,6 +761,12 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
       <c r="C4" t="s">
         <v>38</v>
       </c>
@@ -775,67 +811,310 @@
     <hyperlink ref="H4" r:id="rId3" xr:uid="{E3712C35-31B1-4568-ACCA-825058DDB02A}"/>
     <hyperlink ref="A2" r:id="rId4" xr:uid="{DA6005D3-40BA-468C-B0E8-9B52B3B7A708}"/>
     <hyperlink ref="A3" r:id="rId5" xr:uid="{42E2D2E4-CF79-469E-984E-85EA59A52D8B}"/>
+    <hyperlink ref="A4" r:id="rId6" xr:uid="{46A1C7AD-7E32-4162-83D8-47889FDB6FAE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2143B06A-B04F-4694-90E1-F522012133B7}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N3" sqref="A1:N3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="2" width="23.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="9.06640625" style="2"/>
+    <col min="11" max="11" width="13.265625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.06640625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{493090DD-62F2-4E87-979F-DD08279B1309}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{75A403F7-989F-4FD9-B709-7A32C400CF06}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{B0AB60CC-0512-4777-B92C-6EC2ABD99C1B}"/>
+    <hyperlink ref="A3" r:id="rId4" xr:uid="{F67BCD4A-A8DB-4754-AAB7-5B02E969C95B}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{F77BB9DA-D7D5-46AC-A1F7-B10544534018}"/>
+    <hyperlink ref="B3" r:id="rId6" xr:uid="{6AA1BEFF-25B2-4D27-8051-789FC6908D7B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00B00444-EFD9-469B-A28D-2EA80ABF9796}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="21.59765625" customWidth="1"/>
-    <col min="4" max="4" width="12.53125" customWidth="1"/>
+    <col min="3" max="3" width="14.1328125" customWidth="1"/>
+    <col min="4" max="4" width="13.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{68629369-E24A-42A7-BAD5-3D311C2A1A0C}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{656BEA59-EE49-4B49-8C49-44613E025BFE}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{2B882675-BC3A-44DA-A0C9-4F5470908CE2}"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{68629369-E24A-42A7-BAD5-3D311C2A1A0C}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{656BEA59-EE49-4B49-8C49-44613E025BFE}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{2B882675-BC3A-44DA-A0C9-4F5470908CE2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B14C5A36-8CF4-4A14-8F33-138216C30DA1}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="21.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{C8120E37-417F-48C5-90CA-DE6E162C7B63}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{ECFFE161-6EB7-4EFE-B34D-FC12D5F19C6E}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{44200B56-0D2C-46F7-969D-568EBD17F4E5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>